<commit_message>
Updated the excel dataset
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
+++ b/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528116\Documents\43663 DotNetProjects\WS02_PlanYourDegree\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528116\Documents\43663 DotNetProjects\WS02_PlanYourDegree\PlanYourDegree.Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
-  <si>
-    <t>DegreeAbrev (U Max6)</t>
-  </si>
-  <si>
-    <t>DegreeName (Max 20)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>ACS+2</t>
   </si>
@@ -333,6 +327,12 @@
   </si>
   <si>
     <t xml:space="preserve">DegreeID </t>
+  </si>
+  <si>
+    <t>DegreeAbrev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DegreeName </t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,26 +704,27 @@
     <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="68.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -731,20 +732,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;E2</f>
-        <v>new Degree{DegreeID =1},</v>
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
+        <v>new Degree{DegreeID =1,DegreeAbrev=ACS+2,DegreeName =MS ACS + 2},</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,10 +753,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
+        <v>new Degree{DegreeID =2,DegreeAbrev=ACS+DB,DegreeName =MS ACS + DB},</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,10 +774,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree{DegreeID =3,DegreeAbrev=ACS+NF,DegreeName =MS ACS + NF},</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,10 +795,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree{DegreeID =4,DegreeAbrev=ACS,DegreeName =MS ACS},</v>
       </c>
     </row>
   </sheetData>
@@ -803,13 +834,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -817,10 +848,10 @@
         <v>460</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -828,10 +859,10 @@
         <v>356</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -839,10 +870,10 @@
         <v>542</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -850,10 +881,10 @@
         <v>563</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -861,10 +892,10 @@
         <v>560</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -872,10 +903,10 @@
         <v>555</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -883,10 +914,10 @@
         <v>618</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -894,10 +925,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -905,10 +936,10 @@
         <v>664</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -916,10 +947,10 @@
         <v>691</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -927,10 +958,10 @@
         <v>692</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -938,10 +969,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -949,10 +980,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -978,13 +1009,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,16 +1172,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3087,19 +3118,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3113,10 +3144,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3130,10 +3161,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3147,10 +3178,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3164,10 +3195,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3181,10 +3212,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3198,10 +3229,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3215,10 +3246,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3232,10 +3263,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3249,10 +3280,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3266,10 +3297,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3283,10 +3314,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3300,10 +3331,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3317,10 +3348,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3334,10 +3365,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3351,10 +3382,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3368,10 +3399,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3385,10 +3416,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3402,10 +3433,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3419,10 +3450,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3436,10 +3467,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3453,10 +3484,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3470,10 +3501,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3487,10 +3518,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3504,10 +3535,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3521,10 +3552,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3552,19 +3583,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,10 +3609,10 @@
         <v>528116</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,10 +3626,10 @@
         <v>528116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,10 +3643,10 @@
         <v>530473</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,10 +3660,10 @@
         <v>530473</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3646,10 +3677,10 @@
         <v>533909</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3663,10 +3694,10 @@
         <v>533909</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3680,10 +3711,10 @@
         <v>533570</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3697,10 +3728,10 @@
         <v>533570</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3714,10 +3745,10 @@
         <v>531372</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3731,10 +3762,10 @@
         <v>531372</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3764,16 +3795,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3781,13 +3812,13 @@
         <v>528116</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3795,10 +3826,10 @@
         <v>530473</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3806,10 +3837,10 @@
         <v>533909</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4" s="1">
         <v>919570037</v>
@@ -3820,10 +3851,10 @@
         <v>533570</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="1">
         <v>919569706</v>
@@ -3834,10 +3865,10 @@
         <v>531372</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the sample data set for sql queries for course table Add the course domain model, Register the course context and initialize the db with test data.
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
+++ b/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
   <si>
     <t>ACS+2</t>
   </si>
@@ -59,15 +59,6 @@
     <t>MS ACS</t>
   </si>
   <si>
-    <t>RequirementID (Max 3, Key)</t>
-  </si>
-  <si>
-    <t>RequirementAbbrev (U, Max 10, R)</t>
-  </si>
-  <si>
-    <t>RequirementName (Max 50, R)</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -146,18 +137,12 @@
     <t>20 Advisor Approved Elective-II</t>
   </si>
   <si>
-    <t>DegreeRequirementID (Key)</t>
-  </si>
-  <si>
     <t>DegreeID (FKey-DegreeID)</t>
   </si>
   <si>
     <t>CoruseRequirementID (FKey-CourseID)</t>
   </si>
   <si>
-    <t>DegreeTermRequirementID (Key)</t>
-  </si>
-  <si>
     <t>DegreePlanID (FKey-DegreePlanID)</t>
   </si>
   <si>
@@ -248,9 +233,6 @@
     <t>SP21</t>
   </si>
   <si>
-    <t>DegreePlanId (Key)</t>
-  </si>
-  <si>
     <t>StrudentID (FKey-Student)</t>
   </si>
   <si>
@@ -272,9 +254,6 @@
     <t>Complete the degree Economically</t>
   </si>
   <si>
-    <t>StudentID (Key, Max 6, Min 6)</t>
-  </si>
-  <si>
     <t>First (Max 20)</t>
   </si>
   <si>
@@ -333,6 +312,36 @@
   </si>
   <si>
     <t xml:space="preserve">DegreeName </t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>new Course{</t>
+  </si>
+  <si>
+    <t>CourseID</t>
+  </si>
+  <si>
+    <t>DegreeReqID</t>
+  </si>
+  <si>
+    <t>DegreeTermReqID</t>
+  </si>
+  <si>
+    <t>DegreePlanID</t>
+  </si>
+  <si>
+    <t>StudentID</t>
+  </si>
+  <si>
+    <t>CourseAbbrev</t>
+  </si>
+  <si>
+    <t>CourseName</t>
   </si>
 </sst>
 </file>
@@ -696,7 +705,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,19 +721,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,13 +747,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1" t="str">
-        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
+        <f t="shared" ref="F2:F5" si="0">D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
         <v>new Degree{DegreeID =1,DegreeAbrev=ACS+2,DegreeName =MS ACS + 2},</v>
       </c>
     </row>
@@ -759,13 +768,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F5" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
+        <f t="shared" si="0"/>
         <v>new Degree{DegreeID =2,DegreeAbrev=ACS+DB,DegreeName =MS ACS + DB},</v>
       </c>
     </row>
@@ -780,10 +789,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -801,10 +810,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -818,172 +827,311 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="47" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="91.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>460</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;B2&amp;", "&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
+        <v>new Course{CourseID=460, CourseAbbrev=DB, CourseName=44-460 Database Systems},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>356</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f t="shared" ref="F3:F14" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;B3&amp;", "&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
+        <v>new Course{CourseID=356, CourseAbbrev=NF, CourseName=44-356 Network Fundamentals},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>542</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=542, CourseAbbrev=OOP, CourseName=44-542 Object-Oriented Programming},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>563</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=563, CourseAbbrev=WebApps, CourseName=44-563 Developing Web Applications and Services},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>560</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=560, CourseAbbrev=ADB, CourseName=44-560 Advanced Topics in Database Systems},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>555</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=555, CourseAbbrev=NS, CourseName=44-555 Network Security},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>618</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=618, CourseAbbrev=PM, CourseName=44-618 Project Management in Business and Technology},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=1, CourseAbbrev=Moblie, CourseName=1 	Mobile Computing},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>664</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=664, CourseAbbrev=UX, CourseName=44-664 User Experience Design},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>691</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=691, CourseAbbrev=GDP1, CourseName=44-694 CS Graduate Directed Project I},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>692</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=692, CourseAbbrev=GDP2, CourseName=44-692 CS Graduate Directed Project II},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=10, CourseAbbrev=Elective 1, CourseName=10 Advisor Approved Elective-I},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>new Course{CourseID=20, CourseAbbrev=Elective 2, CourseName=20 Advisor Approved Elective-II},</v>
       </c>
     </row>
   </sheetData>
@@ -995,9 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1009,13 +1155,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1159,9 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1172,16 +1316,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3118,19 +3262,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3144,10 +3288,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3161,10 +3305,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3178,10 +3322,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3195,10 +3339,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3212,10 +3356,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3229,10 +3373,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3246,10 +3390,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3263,10 +3407,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3280,10 +3424,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3297,10 +3441,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3314,10 +3458,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3331,10 +3475,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3348,10 +3492,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3365,10 +3509,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3382,10 +3526,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3399,10 +3543,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3416,10 +3560,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3433,10 +3577,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,10 +3594,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3467,10 +3611,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3484,10 +3628,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3501,10 +3645,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3518,10 +3662,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3535,10 +3679,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3552,10 +3696,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3567,9 +3711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3583,19 +3725,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3609,10 +3751,10 @@
         <v>528116</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3626,10 +3768,10 @@
         <v>528116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3643,10 +3785,10 @@
         <v>530473</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3660,10 +3802,10 @@
         <v>530473</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3677,10 +3819,10 @@
         <v>533909</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3694,10 +3836,10 @@
         <v>533909</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3711,10 +3853,10 @@
         <v>533570</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3728,10 +3870,10 @@
         <v>533570</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3745,10 +3887,10 @@
         <v>531372</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3762,10 +3904,10 @@
         <v>531372</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3778,7 +3920,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3795,16 +3937,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,13 +3954,13 @@
         <v>528116</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3826,10 +3968,10 @@
         <v>530473</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3837,10 +3979,10 @@
         <v>533909</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1">
         <v>919570037</v>
@@ -3851,10 +3993,10 @@
         <v>533570</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1">
         <v>919569706</v>
@@ -3865,10 +4007,10 @@
         <v>531372</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commited work on degree requirement
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
+++ b/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528116\Documents\43663 DotNetProjects\WS02_PlanYourDegree\PlanYourDegree.Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533570\Documents\44663\ws02_Raptors\PlanYourDegree.Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>DegreeID (FKey-DegreeID)</t>
   </si>
   <si>
-    <t>CoruseRequirementID (FKey-CourseID)</t>
-  </si>
-  <si>
     <t>DegreePlanID (FKey-DegreePlanID)</t>
   </si>
   <si>
@@ -342,6 +339,9 @@
   </si>
   <si>
     <t>CourseName</t>
+  </si>
+  <si>
+    <t>CourseID (FKey-CourseID)</t>
   </si>
 </sst>
 </file>
@@ -704,7 +704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -721,19 +721,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F2" s="1" t="str">
         <f t="shared" ref="F2:F5" si="0">D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -768,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -789,10 +789,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -810,10 +810,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -829,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
@@ -846,19 +846,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,10 +872,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;B2&amp;", "&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -893,10 +893,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" ref="F3:F14" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;B3&amp;", "&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
@@ -914,10 +914,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -935,10 +935,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -956,10 +956,10 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -977,10 +977,10 @@
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -998,10 +998,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1019,10 +1019,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1040,10 +1040,10 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1061,10 +1061,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1082,10 +1082,10 @@
         <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1103,10 +1103,10 @@
         <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1124,10 +1124,10 @@
         <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1143,25 +1143,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,22 +1312,24 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="45.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3248,33 +3252,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3288,10 +3293,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3305,10 +3310,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3322,10 +3327,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3339,10 +3344,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3356,10 +3361,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3373,10 +3378,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3390,10 +3395,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,10 +3412,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,10 +3429,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3441,10 +3446,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3458,10 +3463,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3475,10 +3480,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3492,10 +3497,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3509,10 +3514,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3526,10 +3531,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3543,10 +3548,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3560,10 +3565,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3577,10 +3582,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3594,10 +3599,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3611,10 +3616,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3628,10 +3633,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3645,10 +3650,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3662,10 +3667,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3679,10 +3684,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3696,10 +3701,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3716,28 +3721,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3751,10 +3756,10 @@
         <v>528116</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3768,10 +3773,10 @@
         <v>528116</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3785,10 +3790,10 @@
         <v>530473</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3802,10 +3807,10 @@
         <v>530473</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3819,10 +3824,10 @@
         <v>533909</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3836,10 +3841,10 @@
         <v>533909</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3853,10 +3858,10 @@
         <v>533570</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3870,10 +3875,10 @@
         <v>533570</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3887,10 +3892,10 @@
         <v>531372</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3904,10 +3909,10 @@
         <v>531372</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3937,16 +3942,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3954,13 +3959,13 @@
         <v>528116</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3968,10 +3973,10 @@
         <v>530473</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3979,10 +3984,10 @@
         <v>533909</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D4" s="1">
         <v>919570037</v>
@@ -3993,10 +3998,10 @@
         <v>533570</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="D5" s="1">
         <v>919569706</v>
@@ -4007,10 +4012,10 @@
         <v>531372</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the StudentTermID FK on DegreePlan table. Change the database name.
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
+++ b/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533570\Documents\44663\ws02_Raptors\PlanYourDegree.Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528116\Documents\43663 DotNetProjects\WS02_PlanYourDegree\PlanYourDegree.Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="103">
   <si>
     <t>ACS+2</t>
   </si>
@@ -143,18 +143,9 @@
     <t>DegreePlanID (FKey-DegreePlanID)</t>
   </si>
   <si>
-    <t>TermID (FKey-StudentTermID)</t>
-  </si>
-  <si>
     <t>CourseId(FKey-CourseID)</t>
   </si>
   <si>
-    <t>StudentTermId (Key)</t>
-  </si>
-  <si>
-    <t>StudentID (FKey-Student)</t>
-  </si>
-  <si>
     <t>Term </t>
   </si>
   <si>
@@ -345,6 +336,12 @@
   </si>
   <si>
     <t>new DegreeReq{</t>
+  </si>
+  <si>
+    <t>StudentTermID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StudentTermID </t>
   </si>
 </sst>
 </file>
@@ -724,19 +721,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -750,10 +747,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="str">
         <f t="shared" ref="F2:F5" si="0">D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -771,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -792,10 +789,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -813,10 +810,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -849,19 +846,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,10 +872,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;", "&amp;$B$1&amp;"="&amp;B2&amp;", "&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -896,10 +893,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" ref="F3:F14" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;", "&amp;$B$1&amp;"="&amp;B3&amp;", "&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
@@ -917,10 +914,10 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -938,10 +935,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -959,10 +956,10 @@
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -980,10 +977,10 @@
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1001,10 +998,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1022,10 +1019,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1043,10 +1040,10 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1064,10 +1061,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1085,10 +1082,10 @@
         <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1106,10 +1103,10 @@
         <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1127,10 +1124,10 @@
         <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1146,7 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F13"/>
     </sheetView>
   </sheetViews>
@@ -1163,13 +1160,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1183,10 +1180,10 @@
         <v>460</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>D2&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;E2</f>
@@ -1204,10 +1201,10 @@
         <v>542</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="str">
         <f t="shared" ref="F3:F13" si="0">D3&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;E3</f>
@@ -1225,10 +1222,10 @@
         <v>563</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1246,10 +1243,10 @@
         <v>560</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1267,10 +1264,10 @@
         <v>555</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1288,10 +1285,10 @@
         <v>618</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1309,10 +1306,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1330,10 +1327,10 @@
         <v>664</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1351,10 +1348,10 @@
         <v>691</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1372,10 +1369,10 @@
         <v>692</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1393,10 +1390,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1414,10 +1411,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1433,7 +1430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1446,16 +1445,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3378,8 +3377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3393,19 +3392,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3419,10 +3418,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3436,10 +3435,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3453,10 +3452,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3470,10 +3469,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3487,10 +3486,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3504,10 +3503,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3521,10 +3520,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3538,10 +3537,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,10 +3554,10 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3572,10 +3571,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3589,10 +3588,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3606,10 +3605,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3623,10 +3622,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3640,10 +3639,10 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3657,10 +3656,10 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3674,10 +3673,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3691,10 +3690,10 @@
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3708,10 +3707,10 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3725,10 +3724,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3742,10 +3741,10 @@
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3759,10 +3758,10 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3776,10 +3775,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3793,10 +3792,10 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3810,10 +3809,10 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3827,10 +3826,10 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3856,19 +3855,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3882,10 +3881,10 @@
         <v>528116</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,10 +3898,10 @@
         <v>528116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3916,10 +3915,10 @@
         <v>530473</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3933,10 +3932,10 @@
         <v>530473</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3950,10 +3949,10 @@
         <v>533909</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3967,10 +3966,10 @@
         <v>533909</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3984,10 +3983,10 @@
         <v>533570</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -4001,10 +4000,10 @@
         <v>533570</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -4018,10 +4017,10 @@
         <v>531372</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4035,10 +4034,10 @@
         <v>531372</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4068,16 +4067,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4085,13 +4084,13 @@
         <v>528116</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4099,10 +4098,10 @@
         <v>530473</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,10 +4109,10 @@
         <v>533909</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1">
         <v>919570037</v>
@@ -4124,10 +4123,10 @@
         <v>533570</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1">
         <v>919569706</v>
@@ -4138,10 +4137,10 @@
         <v>531372</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sorting and searching to the degrees view
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
+++ b/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="130">
   <si>
     <t>ACS+2</t>
   </si>
@@ -342,9 +342,6 @@
     <t>StudentTermID</t>
   </si>
   <si>
-    <t xml:space="preserve">StudentTermID </t>
-  </si>
-  <si>
     <t>TermId</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>Summer 2024</t>
+  </si>
+  <si>
+    <t>new Term{</t>
   </si>
 </sst>
 </file>
@@ -1512,7 +1512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1826,7 +1826,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,29 +2287,39 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2319,8 +2329,18 @@
       <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="str">
+        <f>D2&amp;$A$1&amp;" = "&amp;A2&amp;" , "&amp;$B$1&amp;" = "&amp;CHAR(34)&amp;B2&amp;CHAR(34)&amp;" , "&amp;$C$1&amp;" = "&amp;CHAR(34)&amp;C2&amp;CHAR(34)&amp;E2</f>
+        <v>new Term{TermId = 1 , TermAbbrev = "F17" , TermName = "Fall 2017"},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2330,8 +2350,18 @@
       <c r="C3" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F22" si="0">D3&amp;$A$1&amp;" = "&amp;A3&amp;" , "&amp;$B$1&amp;" = "&amp;CHAR(34)&amp;B3&amp;CHAR(34)&amp;" , "&amp;$C$1&amp;" = "&amp;CHAR(34)&amp;C3&amp;CHAR(34)&amp;E3</f>
+        <v>new Term{TermId = 2 , TermAbbrev = "SP18" , TermName = "Spring 2018"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2341,8 +2371,18 @@
       <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 3 , TermAbbrev = "SU18" , TermName = "Summer 2018"},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2352,8 +2392,18 @@
       <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 4 , TermAbbrev = "F18" , TermName = "Fall 2018"},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2363,19 +2413,39 @@
       <c r="C6" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 5 , TermAbbrev = "SP19" , TermName = "Spring 2019"},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 6 , TermAbbrev = "Su19" , TermName = "Summer 2019"},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2385,30 +2455,60 @@
       <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 7 , TermAbbrev = "F19" , TermName = "Fall 2019"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 8 , TermAbbrev = "Sp20" , TermName = "Spring 2020"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 9 , TermAbbrev = "Su20" , TermName = "Summer 2020"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2418,126 +2518,246 @@
       <c r="C11" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 10 , TermAbbrev = "F20" , TermName = "Fall 2020"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 11 , TermAbbrev = "Sp21" , TermName = "Spring 2021"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 12 , TermAbbrev = "Su21" , TermName = "Summer 2021"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 13 , TermAbbrev = "F21" , TermName = "Fall 2021"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 14 , TermAbbrev = "Sp22" , TermName = "Spring 2022"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 15 , TermAbbrev = "Su22" , TermName = "Summer 2022"},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 16 , TermAbbrev = "F22" , TermName = "Fall 2022"},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 17 , TermAbbrev = "Sp23" , TermName = "Spring 2023"},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 18 , TermAbbrev = "SU23" , TermName = "Summer 2023"},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="D20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 19 , TermAbbrev = "F23" , TermName = "Fall 2023"},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="D21" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 20 , TermAbbrev = "Sp24" , TermName = "Spring 2024"},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
         <v>129</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>new Term{TermId = 21 , TermAbbrev = "Su24" , TermName = "Summer 2024"},</v>
       </c>
     </row>
   </sheetData>
@@ -2550,7 +2770,7 @@
   <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DegreeReq model and sample data updated Degree controller and detail view updated
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
+++ b/PlanYourDegree.Docs/WS02_PYD_SampleData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -786,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -912,7 +912,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>